<commit_message>
Thankyou page construction and ready to test
</commit_message>
<xml_diff>
--- a/testautomation/src/main/resources/SourceDataFiles/LocatorsGenerated.xlsx
+++ b/testautomation/src/main/resources/SourceDataFiles/LocatorsGenerated.xlsx
@@ -20,26 +20,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">Locator</t>
   </si>
   <si>
     <t xml:space="preserve">Date</t>
   </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -99,8 +104,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -121,23 +130,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added functionality to save locator in external Excel File, start creating datepicker function
</commit_message>
<xml_diff>
--- a/testautomation/src/main/resources/SourceDataFiles/LocatorsGenerated.xlsx
+++ b/testautomation/src/main/resources/SourceDataFiles/LocatorsGenerated.xlsx
@@ -20,15 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t xml:space="preserve">Locator</t>
   </si>
   <si>
     <t xml:space="preserve">Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3</t>
   </si>
 </sst>
 </file>
@@ -130,10 +127,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -149,11 +146,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>